<commit_message>
added images, modified vba modules
</commit_message>
<xml_diff>
--- a/calculadora_hipoteca.xlsx
+++ b/calculadora_hipoteca.xlsx
@@ -8,36 +8,95 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maite\Desktop\maitelizarraga.github.io\calculadora_hipoteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C87D5443-2886-4552-B573-EB1660080338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45749094-75A9-445E-B286-293EE5347B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculadora_Hipoteca" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+  <si>
+    <t>Tipo de interés anual (%)</t>
+  </si>
+  <si>
+    <t>Saldo actual (€)</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>Intereses</t>
+  </si>
+  <si>
+    <t>Desglose</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Cuota</t>
+  </si>
+  <si>
+    <t>Saldo Pendiente</t>
+  </si>
+  <si>
+    <t>Meses restantes hasta revisión anual</t>
+  </si>
+  <si>
+    <t>Meses restantes hasta el final del crédito</t>
+  </si>
+  <si>
+    <t>470,03</t>
+  </si>
+  <si>
+    <t>0,00</t>
+  </si>
+  <si>
+    <t>69227,39</t>
+  </si>
+  <si>
+    <t>68757,36</t>
+  </si>
+  <si>
+    <t>68287,33</t>
+  </si>
+  <si>
+    <t>67817,30</t>
+  </si>
+  <si>
+    <t>67347,28</t>
+  </si>
+  <si>
+    <t>66877,25</t>
+  </si>
+  <si>
+    <t>66407,22</t>
+  </si>
+  <si>
+    <t>65937,19</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +104,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="53"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -62,14 +157,151 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -83,6 +315,227 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>342900</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>99060</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aptos Narrow"/>
+                </a:rPr>
+                <a:t>Calcular Cuota Mensual</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>342900</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>99060</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Button 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92E4DEB2-DE55-9A96-FE6A-AB1352945FC7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aptos Narrow"/>
+                </a:rPr>
+                <a:t>Ver Desglose y Actualización Saldo</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>342900</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>68580</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>1684020</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Button 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32E73B76-6318-EE06-0D81-BF7A0E51F490}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="FF6600"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aptos Narrow"/>
+                </a:rPr>
+                <a:t>Limpiar</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,16 +854,374 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>69697.42</v>
+      </c>
+      <c r="D3" s="15">
+        <v>470.02885739905895</v>
+      </c>
+      <c r="E3" s="16">
+        <v>150.46618669905899</v>
+      </c>
+      <c r="F3" s="17">
+        <v>319.56267069999996</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>5.5019999999999998</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8">
+        <v>249</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8">
+        <v>8</v>
+      </c>
+      <c r="D6" s="19">
+        <v>1</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="7"/>
+      <c r="D7" s="19">
+        <v>2</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="D8" s="19">
+        <v>3</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="19">
+        <v>4</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="D10" s="19">
+        <v>5</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="D11" s="19">
+        <v>6</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D12" s="19">
+        <v>7</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D13" s="19">
+        <v>8</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId4" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!CalcularCuotaMensual.CalcularCuotaMensual">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>342900</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>99060</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId5" name="Button 2">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!CalcularAmortizacion.CalcularAmortizacion">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>342900</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>99060</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId6" name="Button 3">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!LimpiarDatos.LimpiarDatos">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>342900</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>68580</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>1684020</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>144780</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modifications and new images
</commit_message>
<xml_diff>
--- a/calculadora_hipoteca.xlsx
+++ b/calculadora_hipoteca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maite\Desktop\maitelizarraga.github.io\calculadora_hipoteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45749094-75A9-445E-B286-293EE5347B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2B02DF-356D-4BA3-88C7-2FFB7220F180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Tipo de interés anual (%)</t>
   </si>
   <si>
     <t>Saldo actual (€)</t>
+  </si>
+  <si>
+    <t>Cuota Mensual</t>
   </si>
   <si>
     <t>Principal</t>
@@ -39,16 +42,10 @@
     <t>Intereses</t>
   </si>
   <si>
-    <t>Desglose</t>
-  </si>
-  <si>
     <t>Mes</t>
   </si>
   <si>
     <t>Cuota</t>
-  </si>
-  <si>
-    <t>Saldo Pendiente</t>
   </si>
   <si>
     <t>Meses restantes hasta revisión anual</t>
@@ -57,46 +54,27 @@
     <t>Meses restantes hasta el final del crédito</t>
   </si>
   <si>
-    <t>470,03</t>
+    <t>Saldo restante</t>
   </si>
   <si>
-    <t>0,00</t>
+    <t>Rellenar</t>
   </si>
   <si>
-    <t>69227,39</t>
+    <t>↓</t>
   </si>
   <si>
-    <t>68757,36</t>
-  </si>
-  <si>
-    <t>68287,33</t>
-  </si>
-  <si>
-    <t>67817,30</t>
-  </si>
-  <si>
-    <t>67347,28</t>
-  </si>
-  <si>
-    <t>66877,25</t>
-  </si>
-  <si>
-    <t>66407,22</t>
-  </si>
-  <si>
-    <t>65937,19</t>
+    <t>Datos iniciales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
     <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +98,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +119,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +137,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,17 +265,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -298,7 +294,17 @@
     <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -859,7 +865,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,264 +874,275 @@
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
     <col min="3" max="3" width="3.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20">
+        <v>54657</v>
+      </c>
+      <c r="D3" s="13">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="E3" s="14">
+        <v>196.04896866197473</v>
+      </c>
+      <c r="F3" s="15">
+        <v>250.60234499999999</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="20">
+        <v>5.5019999999999998</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="20">
+        <v>180</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="F5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="B6" s="20">
+        <v>8</v>
+      </c>
+      <c r="D6" s="17">
+        <v>1</v>
+      </c>
+      <c r="E6" s="19">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="F6" s="19">
+        <v>196.04896866197473</v>
+      </c>
+      <c r="G6" s="19">
+        <v>250.60234499999999</v>
+      </c>
+      <c r="H6" s="19">
+        <v>54460.951031338023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="D7" s="17">
         <v>2</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="E7" s="19">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="F7" s="19">
+        <v>196.94785318328988</v>
+      </c>
+      <c r="G7" s="19">
+        <v>249.70346047868483</v>
+      </c>
+      <c r="H7" s="19">
+        <v>54264.003178154737</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="D8" s="17">
         <v>3</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8">
-        <v>69697.42</v>
-      </c>
-      <c r="D3" s="15">
-        <v>470.02885739905895</v>
-      </c>
-      <c r="E3" s="16">
-        <v>150.46618669905899</v>
-      </c>
-      <c r="F3" s="17">
-        <v>319.56267069999996</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="8">
-        <v>5.5019999999999998</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="8">
-        <v>249</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="E8" s="19">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="F8" s="19">
+        <v>197.85085909013526</v>
+      </c>
+      <c r="G8" s="19">
+        <v>248.80045457183945</v>
+      </c>
+      <c r="H8" s="19">
+        <v>54066.152319064604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="17">
         <v>4</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="E9" s="19">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="F9" s="19">
+        <v>198.75800527906352</v>
+      </c>
+      <c r="G9" s="19">
+        <v>247.89330838291119</v>
+      </c>
+      <c r="H9" s="19">
+        <v>53867.394313785539</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="D10" s="17">
+        <v>5</v>
+      </c>
+      <c r="E10" s="19">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="F10" s="19">
+        <v>199.66931073326805</v>
+      </c>
+      <c r="G10" s="19">
+        <v>246.98200292870666</v>
+      </c>
+      <c r="H10" s="19">
+        <v>53667.72500305227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="D11" s="17">
+        <v>6</v>
+      </c>
+      <c r="E11" s="19">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="F11" s="19">
+        <v>200.58479452298008</v>
+      </c>
+      <c r="G11" s="19">
+        <v>246.06651913899464</v>
+      </c>
+      <c r="H11" s="19">
+        <v>53467.140208529287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D12" s="17">
+        <v>7</v>
+      </c>
+      <c r="E12" s="19">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="F12" s="19">
+        <v>201.50447580586794</v>
+      </c>
+      <c r="G12" s="19">
+        <v>245.14683785610677</v>
+      </c>
+      <c r="H12" s="19">
+        <v>53265.635732723422</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D13" s="17">
         <v>8</v>
       </c>
-      <c r="B6" s="8">
-        <v>8</v>
-      </c>
-      <c r="D6" s="19">
-        <v>1</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="7"/>
-      <c r="D7" s="19">
-        <v>2</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="D8" s="19">
-        <v>3</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="19">
-        <v>4</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="D10" s="19">
-        <v>5</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="D11" s="19">
-        <v>6</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="19">
-        <v>7</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D13" s="19">
-        <v>8</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>19</v>
+      <c r="E13" s="19">
+        <v>446.65131366197471</v>
+      </c>
+      <c r="F13" s="19">
+        <v>202.42837382743784</v>
+      </c>
+      <c r="G13" s="19">
+        <v>244.22293983453687</v>
+      </c>
+      <c r="H13" s="19">
+        <v>53063.207358895983</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" s="2"/>

</xml_diff>

<commit_message>
added banner to readme
</commit_message>
<xml_diff>
--- a/calculadora_hipoteca.xlsx
+++ b/calculadora_hipoteca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maite\Desktop\maitelizarraga.github.io\calculadora_hipoteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2B02DF-356D-4BA3-88C7-2FFB7220F180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60454B25-EC28-438D-8493-FA4C79853F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -865,7 +865,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>